<commit_message>
Refactored base js file
</commit_message>
<xml_diff>
--- a/src/test/TestConditions.xlsx
+++ b/src/test/TestConditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Documents\Homework\ECSE428 - Software Practice\Assignment B\repo\ECSE428_ASSB_G49\src\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1083D031-8DD6-4C8E-A99F-1D716CCF94F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586C3FAD-F51D-4DE9-88C6-1D1230E58529}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30450" yWindow="2325" windowWidth="15675" windowHeight="15555" xr2:uid="{AB891CDE-DAF3-4AA3-92BD-6DBF6800CE47}"/>
+    <workbookView xWindow="4530" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{AB891CDE-DAF3-4AA3-92BD-6DBF6800CE47}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis" sheetId="1" r:id="rId1"/>
@@ -346,9 +346,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -366,9 +363,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -385,6 +379,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -703,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238D5791-8EED-4FC6-B7FB-0F4224317556}">
   <dimension ref="A1:AR29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -717,100 +717,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>-1</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="13">
+      <c r="B2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="12">
         <v>-1</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="13">
+      <c r="D2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="12">
         <v>-1</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="1">
         <v>200</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="10">
         <v>0.49</v>
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
+      <c r="A3" s="18">
         <v>0</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="19">
+      <c r="B3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="18">
         <v>0</v>
       </c>
-      <c r="D3" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="19">
+      <c r="D3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="18">
         <v>0</v>
       </c>
-      <c r="F3" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="13">
+      <c r="F3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="12">
         <v>400</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+      <c r="A4" s="18">
         <v>1</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="19">
+      <c r="B4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="18">
         <v>1</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="19">
+      <c r="D4" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="18">
         <v>1</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="1"/>
@@ -819,26 +819,26 @@
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="19">
+      <c r="A5" s="18">
         <v>139</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="19">
+      <c r="B5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="18">
         <v>89</v>
       </c>
-      <c r="D5" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="19">
+      <c r="D5" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="18">
         <v>2</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="18">
+      <c r="H5" s="17">
         <v>2.4</v>
       </c>
       <c r="Z5" s="4" t="s">
@@ -901,7 +901,7 @@
         <v>14</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
         <v>18</v>
       </c>
       <c r="Z6" s="4" t="s">
@@ -945,10 +945,10 @@
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="A7" s="20">
         <v>141</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1">
@@ -963,10 +963,10 @@
       <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="38"/>
       <c r="Z7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1026,10 +1026,10 @@
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="A8" s="20">
         <v>244</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1">
@@ -1044,10 +1044,10 @@
       <c r="F8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="28"/>
+      <c r="H8" s="39"/>
       <c r="Z8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1059,10 +1059,10 @@
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+      <c r="A9" s="20">
         <v>245</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="1">
@@ -1077,8 +1077,8 @@
       <c r="F9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
       <c r="Z9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1096,148 +1096,148 @@
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+      <c r="A10" s="18">
         <v>246</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="19">
+      <c r="B10" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="18">
         <v>157</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="23">
+      <c r="D10" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="22">
         <v>31</v>
       </c>
-      <c r="F10" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
+      <c r="F10" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+      <c r="A11" s="18">
         <v>379</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="19">
+      <c r="B11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="18">
         <v>269</v>
       </c>
-      <c r="D11" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="23">
+      <c r="D11" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="22">
         <v>49</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
+      <c r="F11" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="18">
         <v>380</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="19">
+      <c r="B12" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="18">
         <v>270</v>
       </c>
-      <c r="D12" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="23">
+      <c r="D12" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="22">
         <v>50</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
+      <c r="F12" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>381</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="13">
+      <c r="B13" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="12">
         <v>271</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="19">
+      <c r="D13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="18">
         <v>51</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="12">
         <v>-1</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="13">
+      <c r="B14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="12">
         <v>-1</v>
       </c>
-      <c r="D14" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="19">
+      <c r="D14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="18">
         <v>99</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+      <c r="A15" s="18">
         <v>0</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="19">
+      <c r="B15" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="18">
         <v>0</v>
       </c>
-      <c r="D15" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="19">
+      <c r="D15" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="18">
         <v>100</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
+      <c r="A16" s="18">
         <v>1</v>
       </c>
-      <c r="B16" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="19">
+      <c r="B16" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="18">
         <v>1</v>
       </c>
-      <c r="D16" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="25">
+      <c r="D16" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="24">
         <v>101</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="25" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1254,90 +1254,90 @@
       <c r="D17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="24">
         <v>499</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="25" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="18">
         <v>12</v>
       </c>
-      <c r="B18" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="19">
+      <c r="B18" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="18">
         <v>8</v>
       </c>
-      <c r="D18" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="25">
+      <c r="D18" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="24">
         <v>500</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="F18" s="25" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
+      <c r="A19" s="12">
         <v>16</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="13">
+      <c r="B19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="12">
         <v>12</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="13">
+      <c r="D19" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="12">
         <v>501</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+      <c r="A20" s="12">
         <v>0</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="12">
         <v>0</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="12">
         <v>-1</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="32" t="s">
+      <c r="B21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="19">
+      <c r="D21" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="18">
         <v>0</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="19" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1358,50 +1358,50 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E24" s="23">
+      <c r="E24" s="22">
         <v>1.5</v>
       </c>
-      <c r="F24" s="24" t="s">
+      <c r="F24" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="19">
+      <c r="E25" s="18">
         <v>2.5</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="25">
+      <c r="E26" s="24">
         <v>9</v>
       </c>
-      <c r="F26" s="26" t="s">
+      <c r="F26" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E27" s="13">
+      <c r="E27" s="12">
         <v>20</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="13">
+      <c r="E28" s="12">
         <v>0</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="14">
         <v>0</v>
       </c>
     </row>
@@ -1418,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC910C0-C4E2-486F-90F5-9B3D69A286F7}">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,34 +1437,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="32" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1475,10 +1475,10 @@
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="16">
         <v>-1</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="4">
@@ -1507,10 +1507,10 @@
       <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="26">
         <v>0</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="4">
@@ -1539,10 +1539,10 @@
       <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="26">
         <v>1</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="4">
@@ -1571,10 +1571,10 @@
       <c r="B5" s="4">
         <v>4</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="26">
         <v>139</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="4">
@@ -1624,7 +1624,7 @@
       <c r="I6" s="4">
         <v>200</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="10">
         <v>0.49</v>
       </c>
     </row>
@@ -1656,7 +1656,7 @@
       <c r="I7" s="4">
         <v>200</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="10">
         <v>0.49</v>
       </c>
     </row>
@@ -1688,7 +1688,7 @@
       <c r="I8" s="4">
         <v>200</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="10">
         <v>0.49</v>
       </c>
     </row>
@@ -1720,7 +1720,7 @@
       <c r="I9" s="4">
         <v>200</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <v>0.49</v>
       </c>
     </row>
@@ -1731,10 +1731,10 @@
       <c r="B10" s="4">
         <v>9</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="26">
         <v>246</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="26" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="4">
@@ -1763,10 +1763,10 @@
       <c r="B11" s="4">
         <v>10</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="26">
         <v>379</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="26" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="4">
@@ -1795,10 +1795,10 @@
       <c r="B12" s="4">
         <v>11</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="26">
         <v>380</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="26" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="4">
@@ -1827,10 +1827,10 @@
       <c r="B13" s="4">
         <v>12</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="16">
         <v>381</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="4">
@@ -1859,10 +1859,10 @@
       <c r="B14" s="4">
         <v>13</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="16">
         <v>-1</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="4">
@@ -1891,10 +1891,10 @@
       <c r="B15" s="4">
         <v>14</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="26">
         <v>0</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="4">
@@ -1923,10 +1923,10 @@
       <c r="B16" s="4">
         <v>15</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="26">
         <v>1</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="4">
@@ -1987,10 +1987,10 @@
       <c r="B18" s="4">
         <v>17</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="26">
         <v>12</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="4">
@@ -2019,10 +2019,10 @@
       <c r="B19" s="4">
         <v>18</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="16">
         <v>16</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="4">
@@ -2051,10 +2051,10 @@
       <c r="B20" s="4">
         <v>19</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="16">
         <v>0</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="16" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="4">
@@ -2083,10 +2083,10 @@
       <c r="B21" s="4">
         <v>20</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="4">
@@ -2118,13 +2118,13 @@
       <c r="C22" s="4">
         <v>200</v>
       </c>
-      <c r="D22" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="17">
+      <c r="D22" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="16">
         <v>-1</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="16" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="9">
@@ -2150,13 +2150,13 @@
       <c r="C23" s="4">
         <v>200</v>
       </c>
-      <c r="D23" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="27">
+      <c r="D23" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="26">
         <v>0</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="26" t="s">
         <v>11</v>
       </c>
       <c r="G23" s="9">
@@ -2182,13 +2182,13 @@
       <c r="C24" s="4">
         <v>200</v>
       </c>
-      <c r="D24" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="27">
+      <c r="D24" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="26">
         <v>1</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="26" t="s">
         <v>11</v>
       </c>
       <c r="G24" s="9">
@@ -2214,13 +2214,13 @@
       <c r="C25" s="4">
         <v>200</v>
       </c>
-      <c r="D25" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="27">
+      <c r="D25" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="26">
         <v>89</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="26" t="s">
         <v>11</v>
       </c>
       <c r="G25" s="9">
@@ -2246,7 +2246,7 @@
       <c r="C26" s="4">
         <v>200</v>
       </c>
-      <c r="D26" s="36" t="s">
+      <c r="D26" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="4">
@@ -2264,7 +2264,7 @@
       <c r="I26" s="9">
         <v>200</v>
       </c>
-      <c r="J26" s="11">
+      <c r="J26" s="10">
         <v>0.49</v>
       </c>
     </row>
@@ -2278,7 +2278,7 @@
       <c r="C27" s="4">
         <v>200</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="4">
@@ -2296,7 +2296,7 @@
       <c r="I27" s="9">
         <v>200</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J27" s="10">
         <v>0.49</v>
       </c>
     </row>
@@ -2310,7 +2310,7 @@
       <c r="C28" s="4">
         <v>200</v>
       </c>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="4">
@@ -2328,7 +2328,7 @@
       <c r="I28" s="9">
         <v>200</v>
       </c>
-      <c r="J28" s="11">
+      <c r="J28" s="10">
         <v>0.49</v>
       </c>
     </row>
@@ -2342,7 +2342,7 @@
       <c r="C29" s="4">
         <v>200</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="4">
@@ -2360,7 +2360,7 @@
       <c r="I29" s="9">
         <v>200</v>
       </c>
-      <c r="J29" s="11">
+      <c r="J29" s="10">
         <v>0.49</v>
       </c>
     </row>
@@ -2374,13 +2374,13 @@
       <c r="C30" s="4">
         <v>200</v>
       </c>
-      <c r="D30" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="27">
+      <c r="D30" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="26">
         <v>157</v>
       </c>
-      <c r="F30" s="27" t="s">
+      <c r="F30" s="26" t="s">
         <v>11</v>
       </c>
       <c r="G30" s="9">
@@ -2406,13 +2406,13 @@
       <c r="C31" s="4">
         <v>200</v>
       </c>
-      <c r="D31" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="27">
+      <c r="D31" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="26">
         <v>269</v>
       </c>
-      <c r="F31" s="27" t="s">
+      <c r="F31" s="26" t="s">
         <v>11</v>
       </c>
       <c r="G31" s="9">
@@ -2438,13 +2438,13 @@
       <c r="C32" s="4">
         <v>200</v>
       </c>
-      <c r="D32" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="27">
+      <c r="D32" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="26">
         <v>270</v>
       </c>
-      <c r="F32" s="27" t="s">
+      <c r="F32" s="26" t="s">
         <v>11</v>
       </c>
       <c r="G32" s="9">
@@ -2470,13 +2470,13 @@
       <c r="C33" s="4">
         <v>200</v>
       </c>
-      <c r="D33" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="17">
+      <c r="D33" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="16">
         <v>271</v>
       </c>
-      <c r="F33" s="17" t="s">
+      <c r="F33" s="16" t="s">
         <v>11</v>
       </c>
       <c r="G33" s="9">
@@ -2502,13 +2502,13 @@
       <c r="C34" s="4">
         <v>200</v>
       </c>
-      <c r="D34" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="17">
+      <c r="D34" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="16">
         <v>-1</v>
       </c>
-      <c r="F34" s="17" t="s">
+      <c r="F34" s="16" t="s">
         <v>15</v>
       </c>
       <c r="G34" s="9">
@@ -2534,13 +2534,13 @@
       <c r="C35" s="4">
         <v>200</v>
       </c>
-      <c r="D35" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="27">
+      <c r="D35" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="26">
         <v>0</v>
       </c>
-      <c r="F35" s="27" t="s">
+      <c r="F35" s="26" t="s">
         <v>15</v>
       </c>
       <c r="G35" s="9">
@@ -2566,13 +2566,13 @@
       <c r="C36" s="4">
         <v>200</v>
       </c>
-      <c r="D36" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="27">
+      <c r="D36" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="26">
         <v>1</v>
       </c>
-      <c r="F36" s="27" t="s">
+      <c r="F36" s="26" t="s">
         <v>15</v>
       </c>
       <c r="G36" s="9">
@@ -2598,7 +2598,7 @@
       <c r="C37" s="4">
         <v>200</v>
       </c>
-      <c r="D37" s="36" t="s">
+      <c r="D37" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="4">
@@ -2630,13 +2630,13 @@
       <c r="C38" s="4">
         <v>200</v>
       </c>
-      <c r="D38" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="27">
+      <c r="D38" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="26">
         <v>8</v>
       </c>
-      <c r="F38" s="27" t="s">
+      <c r="F38" s="26" t="s">
         <v>15</v>
       </c>
       <c r="G38" s="9">
@@ -2662,13 +2662,13 @@
       <c r="C39" s="4">
         <v>200</v>
       </c>
-      <c r="D39" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="17">
+      <c r="D39" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="16">
         <v>12</v>
       </c>
-      <c r="F39" s="17" t="s">
+      <c r="F39" s="16" t="s">
         <v>15</v>
       </c>
       <c r="G39" s="9">
@@ -2694,13 +2694,13 @@
       <c r="C40" s="4">
         <v>200</v>
       </c>
-      <c r="D40" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="17">
+      <c r="D40" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="16">
         <v>0</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="F40" s="16" t="s">
         <v>26</v>
       </c>
       <c r="G40" s="9">
@@ -2726,13 +2726,13 @@
       <c r="C41" s="4">
         <v>200</v>
       </c>
-      <c r="D41" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="31" t="s">
+      <c r="D41" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="F41" s="16" t="s">
         <v>11</v>
       </c>
       <c r="G41" s="9">
@@ -2758,7 +2758,7 @@
       <c r="C42" s="4">
         <v>200</v>
       </c>
-      <c r="D42" s="36" t="s">
+      <c r="D42" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="4">
@@ -2767,10 +2767,10 @@
       <c r="F42" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G42" s="17">
+      <c r="G42" s="16">
         <v>-1</v>
       </c>
-      <c r="H42" s="17" t="s">
+      <c r="H42" s="16" t="s">
         <v>14</v>
       </c>
       <c r="I42" s="4">
@@ -2790,7 +2790,7 @@
       <c r="C43" s="4">
         <v>200</v>
       </c>
-      <c r="D43" s="36" t="s">
+      <c r="D43" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E43" s="4">
@@ -2799,10 +2799,10 @@
       <c r="F43" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G43" s="27">
+      <c r="G43" s="26">
         <v>0</v>
       </c>
-      <c r="H43" s="27" t="s">
+      <c r="H43" s="26" t="s">
         <v>14</v>
       </c>
       <c r="I43" s="9">
@@ -2822,7 +2822,7 @@
       <c r="C44" s="4">
         <v>200</v>
       </c>
-      <c r="D44" s="36" t="s">
+      <c r="D44" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E44" s="4">
@@ -2831,10 +2831,10 @@
       <c r="F44" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G44" s="27">
+      <c r="G44" s="26">
         <v>1</v>
       </c>
-      <c r="H44" s="27" t="s">
+      <c r="H44" s="26" t="s">
         <v>14</v>
       </c>
       <c r="I44" s="9">
@@ -2854,7 +2854,7 @@
       <c r="C45" s="4">
         <v>200</v>
       </c>
-      <c r="D45" s="36" t="s">
+      <c r="D45" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E45" s="4">
@@ -2863,10 +2863,10 @@
       <c r="F45" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G45" s="27">
+      <c r="G45" s="26">
         <v>2</v>
       </c>
-      <c r="H45" s="27" t="s">
+      <c r="H45" s="26" t="s">
         <v>14</v>
       </c>
       <c r="I45" s="9">
@@ -2886,7 +2886,7 @@
       <c r="C46" s="4">
         <v>200</v>
       </c>
-      <c r="D46" s="36" t="s">
+      <c r="D46" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E46" s="4">
@@ -2904,7 +2904,7 @@
       <c r="I46" s="9">
         <v>200</v>
       </c>
-      <c r="J46" s="11">
+      <c r="J46" s="10">
         <v>0.49</v>
       </c>
     </row>
@@ -2918,7 +2918,7 @@
       <c r="C47" s="4">
         <v>200</v>
       </c>
-      <c r="D47" s="36" t="s">
+      <c r="D47" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="4">
@@ -2936,7 +2936,7 @@
       <c r="I47" s="9">
         <v>200</v>
       </c>
-      <c r="J47" s="11">
+      <c r="J47" s="10">
         <v>0.49</v>
       </c>
     </row>
@@ -2950,7 +2950,7 @@
       <c r="C48" s="4">
         <v>200</v>
       </c>
-      <c r="D48" s="36" t="s">
+      <c r="D48" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E48" s="4">
@@ -2968,7 +2968,7 @@
       <c r="I48" s="9">
         <v>200</v>
       </c>
-      <c r="J48" s="11">
+      <c r="J48" s="10">
         <v>0.49</v>
       </c>
     </row>
@@ -2982,7 +2982,7 @@
       <c r="C49" s="4">
         <v>200</v>
       </c>
-      <c r="D49" s="36" t="s">
+      <c r="D49" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E49" s="4">
@@ -3000,7 +3000,7 @@
       <c r="I49" s="9">
         <v>200</v>
       </c>
-      <c r="J49" s="11">
+      <c r="J49" s="10">
         <v>0.49</v>
       </c>
     </row>
@@ -3014,7 +3014,7 @@
       <c r="C50" s="4">
         <v>200</v>
       </c>
-      <c r="D50" s="36" t="s">
+      <c r="D50" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E50" s="4">
@@ -3023,10 +3023,10 @@
       <c r="F50" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G50" s="29">
+      <c r="G50" s="27">
         <v>31</v>
       </c>
-      <c r="H50" s="29" t="s">
+      <c r="H50" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I50" s="9">
@@ -3046,7 +3046,7 @@
       <c r="C51" s="4">
         <v>200</v>
       </c>
-      <c r="D51" s="36" t="s">
+      <c r="D51" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="4">
@@ -3055,10 +3055,10 @@
       <c r="F51" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G51" s="29">
+      <c r="G51" s="27">
         <v>49</v>
       </c>
-      <c r="H51" s="29" t="s">
+      <c r="H51" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I51" s="9">
@@ -3078,7 +3078,7 @@
       <c r="C52" s="4">
         <v>200</v>
       </c>
-      <c r="D52" s="36" t="s">
+      <c r="D52" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="4">
@@ -3087,10 +3087,10 @@
       <c r="F52" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G52" s="29">
+      <c r="G52" s="27">
         <v>50</v>
       </c>
-      <c r="H52" s="29" t="s">
+      <c r="H52" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I52" s="9">
@@ -3110,7 +3110,7 @@
       <c r="C53" s="4">
         <v>200</v>
       </c>
-      <c r="D53" s="36" t="s">
+      <c r="D53" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E53" s="4">
@@ -3119,10 +3119,10 @@
       <c r="F53" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G53" s="27">
+      <c r="G53" s="26">
         <v>51</v>
       </c>
-      <c r="H53" s="27" t="s">
+      <c r="H53" s="26" t="s">
         <v>14</v>
       </c>
       <c r="I53" s="9">
@@ -3142,7 +3142,7 @@
       <c r="C54" s="4">
         <v>200</v>
       </c>
-      <c r="D54" s="36" t="s">
+      <c r="D54" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E54" s="4">
@@ -3151,10 +3151,10 @@
       <c r="F54" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G54" s="27">
+      <c r="G54" s="26">
         <v>99</v>
       </c>
-      <c r="H54" s="27" t="s">
+      <c r="H54" s="26" t="s">
         <v>14</v>
       </c>
       <c r="I54" s="9">
@@ -3174,7 +3174,7 @@
       <c r="C55" s="4">
         <v>200</v>
       </c>
-      <c r="D55" s="36" t="s">
+      <c r="D55" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E55" s="4">
@@ -3183,10 +3183,10 @@
       <c r="F55" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G55" s="27">
+      <c r="G55" s="26">
         <v>100</v>
       </c>
-      <c r="H55" s="27" t="s">
+      <c r="H55" s="26" t="s">
         <v>14</v>
       </c>
       <c r="I55" s="9">
@@ -3206,7 +3206,7 @@
       <c r="C56" s="4">
         <v>200</v>
       </c>
-      <c r="D56" s="36" t="s">
+      <c r="D56" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E56" s="4">
@@ -3215,10 +3215,10 @@
       <c r="F56" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G56" s="30">
+      <c r="G56" s="28">
         <v>101</v>
       </c>
-      <c r="H56" s="30" t="s">
+      <c r="H56" s="28" t="s">
         <v>14</v>
       </c>
       <c r="I56" s="9">
@@ -3238,7 +3238,7 @@
       <c r="C57" s="4">
         <v>200</v>
       </c>
-      <c r="D57" s="36" t="s">
+      <c r="D57" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E57" s="4">
@@ -3247,10 +3247,10 @@
       <c r="F57" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G57" s="30">
+      <c r="G57" s="28">
         <v>499</v>
       </c>
-      <c r="H57" s="30" t="s">
+      <c r="H57" s="28" t="s">
         <v>14</v>
       </c>
       <c r="I57" s="9">
@@ -3270,7 +3270,7 @@
       <c r="C58" s="4">
         <v>200</v>
       </c>
-      <c r="D58" s="36" t="s">
+      <c r="D58" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E58" s="4">
@@ -3279,10 +3279,10 @@
       <c r="F58" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G58" s="30">
+      <c r="G58" s="28">
         <v>500</v>
       </c>
-      <c r="H58" s="30" t="s">
+      <c r="H58" s="28" t="s">
         <v>14</v>
       </c>
       <c r="I58" s="9">
@@ -3302,7 +3302,7 @@
       <c r="C59" s="4">
         <v>200</v>
       </c>
-      <c r="D59" s="36" t="s">
+      <c r="D59" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E59" s="4">
@@ -3311,10 +3311,10 @@
       <c r="F59" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G59" s="17">
+      <c r="G59" s="16">
         <v>501</v>
       </c>
-      <c r="H59" s="17" t="s">
+      <c r="H59" s="16" t="s">
         <v>14</v>
       </c>
       <c r="I59" s="4">
@@ -3334,7 +3334,7 @@
       <c r="C60" s="4">
         <v>200</v>
       </c>
-      <c r="D60" s="36" t="s">
+      <c r="D60" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E60" s="4">
@@ -3343,10 +3343,10 @@
       <c r="F60" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G60" s="17">
+      <c r="G60" s="16">
         <v>-1</v>
       </c>
-      <c r="H60" s="17" t="s">
+      <c r="H60" s="16" t="s">
         <v>16</v>
       </c>
       <c r="I60" s="4">
@@ -3366,7 +3366,7 @@
       <c r="C61" s="4">
         <v>200</v>
       </c>
-      <c r="D61" s="36" t="s">
+      <c r="D61" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E61" s="4">
@@ -3375,10 +3375,10 @@
       <c r="F61" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G61" s="27">
+      <c r="G61" s="26">
         <v>0</v>
       </c>
-      <c r="H61" s="27" t="s">
+      <c r="H61" s="26" t="s">
         <v>16</v>
       </c>
       <c r="I61" s="9">
@@ -3398,7 +3398,7 @@
       <c r="C62" s="4">
         <v>200</v>
       </c>
-      <c r="D62" s="36" t="s">
+      <c r="D62" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="4">
@@ -3430,7 +3430,7 @@
       <c r="C63" s="4">
         <v>200</v>
       </c>
-      <c r="D63" s="36" t="s">
+      <c r="D63" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E63" s="4">
@@ -3462,7 +3462,7 @@
       <c r="C64" s="4">
         <v>200</v>
       </c>
-      <c r="D64" s="36" t="s">
+      <c r="D64" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E64" s="4">
@@ -3471,10 +3471,10 @@
       <c r="F64" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G64" s="29">
+      <c r="G64" s="27">
         <v>1.5</v>
       </c>
-      <c r="H64" s="29" t="s">
+      <c r="H64" s="27" t="s">
         <v>16</v>
       </c>
       <c r="I64" s="9">
@@ -3494,7 +3494,7 @@
       <c r="C65" s="4">
         <v>200</v>
       </c>
-      <c r="D65" s="36" t="s">
+      <c r="D65" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E65" s="4">
@@ -3503,10 +3503,10 @@
       <c r="F65" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G65" s="27">
+      <c r="G65" s="26">
         <v>2.5</v>
       </c>
-      <c r="H65" s="27" t="s">
+      <c r="H65" s="26" t="s">
         <v>16</v>
       </c>
       <c r="I65" s="9">
@@ -3526,7 +3526,7 @@
       <c r="C66" s="4">
         <v>200</v>
       </c>
-      <c r="D66" s="36" t="s">
+      <c r="D66" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E66" s="4">
@@ -3535,10 +3535,10 @@
       <c r="F66" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G66" s="30">
+      <c r="G66" s="28">
         <v>9</v>
       </c>
-      <c r="H66" s="30" t="s">
+      <c r="H66" s="28" t="s">
         <v>16</v>
       </c>
       <c r="I66" s="9">
@@ -3558,7 +3558,7 @@
       <c r="C67" s="4">
         <v>200</v>
       </c>
-      <c r="D67" s="36" t="s">
+      <c r="D67" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="4">
@@ -3567,10 +3567,10 @@
       <c r="F67" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G67" s="17">
+      <c r="G67" s="16">
         <v>20</v>
       </c>
-      <c r="H67" s="17" t="s">
+      <c r="H67" s="16" t="s">
         <v>16</v>
       </c>
       <c r="I67" s="4">
@@ -3590,7 +3590,7 @@
       <c r="C68" s="4">
         <v>200</v>
       </c>
-      <c r="D68" s="36" t="s">
+      <c r="D68" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="4">
@@ -3599,10 +3599,10 @@
       <c r="F68" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G68" s="17">
+      <c r="G68" s="16">
         <v>0</v>
       </c>
-      <c r="H68" s="17" t="s">
+      <c r="H68" s="16" t="s">
         <v>26</v>
       </c>
       <c r="I68" s="4">
@@ -3622,7 +3622,7 @@
       <c r="C69" s="5">
         <v>200</v>
       </c>
-      <c r="D69" s="38" t="s">
+      <c r="D69" s="36" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="5">
@@ -3631,10 +3631,10 @@
       <c r="F69" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G69" s="39" t="s">
+      <c r="G69" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="H69" s="16">
+      <c r="H69" s="15">
         <v>0</v>
       </c>
       <c r="I69" s="5">

</xml_diff>

<commit_message>
Commit first test. First test not itself tested.
</commit_message>
<xml_diff>
--- a/src/test/TestConditions.xlsx
+++ b/src/test/TestConditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Documents\Homework\ECSE428 - Software Practice\Assignment B\repo\ECSE428_ASSB_G49\src\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586C3FAD-F51D-4DE9-88C6-1D1230E58529}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B85CB22-E969-4389-96F5-2470F79FB9DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4530" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{AB891CDE-DAF3-4AA3-92BD-6DBF6800CE47}"/>
   </bookViews>
@@ -106,22 +106,13 @@
     <t>send.length</t>
   </si>
   <si>
-    <t>send.lengthUnit</t>
-  </si>
-  <si>
     <t>send.width</t>
-  </si>
-  <si>
-    <t>send.widthUnit</t>
   </si>
   <si>
     <t>asdf</t>
   </si>
   <si>
     <t>send.weight</t>
-  </si>
-  <si>
-    <t>send.weightUnit</t>
   </si>
   <si>
     <t>expected.Code</t>
@@ -137,6 +128,15 @@
   </si>
   <si>
     <t>WeightTests</t>
+  </si>
+  <si>
+    <t>send.length_unit</t>
+  </si>
+  <si>
+    <t>send.width_unit</t>
+  </si>
+  <si>
+    <t>send.weight_unit</t>
   </si>
 </sst>
 </file>
@@ -335,7 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -375,7 +375,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -385,6 +384,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -963,10 +974,10 @@
       <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="38"/>
+      <c r="H7" s="37"/>
       <c r="Z7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1044,10 +1055,10 @@
       <c r="F8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="39"/>
+      <c r="H8" s="38"/>
       <c r="Z8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1077,8 +1088,8 @@
       <c r="F9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
       <c r="Z9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1114,8 +1125,8 @@
       <c r="F10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
@@ -1136,8 +1147,8 @@
       <c r="F11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
@@ -1158,8 +1169,8 @@
       <c r="F12" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
@@ -1306,13 +1317,13 @@
         <v>0</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" s="12">
         <v>0</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E20" s="12">
         <v>-1</v>
@@ -1323,13 +1334,13 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>11</v>
@@ -1394,12 +1405,12 @@
         <v>0</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E29" s="30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F29" s="14">
         <v>0</v>
@@ -1419,58 +1430,51 @@
   <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="H1" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="41" t="s">
         <v>27</v>
-      </c>
-      <c r="H1" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1502,7 +1506,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
@@ -1534,7 +1538,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4">
         <v>3</v>
@@ -1566,7 +1570,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
@@ -1598,7 +1602,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4">
         <v>5</v>
@@ -1630,7 +1634,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B7" s="4">
         <v>6</v>
@@ -1662,7 +1666,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" s="4">
         <v>7</v>
@@ -1694,7 +1698,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" s="4">
         <v>8</v>
@@ -1726,7 +1730,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" s="4">
         <v>9</v>
@@ -1758,7 +1762,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B11" s="4">
         <v>10</v>
@@ -1790,7 +1794,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4">
         <v>11</v>
@@ -1822,7 +1826,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" s="4">
         <v>12</v>
@@ -1854,7 +1858,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" s="4">
         <v>13</v>
@@ -1886,7 +1890,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B15" s="4">
         <v>14</v>
@@ -1918,7 +1922,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B16" s="4">
         <v>15</v>
@@ -1950,7 +1954,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" s="4">
         <v>16</v>
@@ -1982,7 +1986,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B18" s="4">
         <v>17</v>
@@ -2014,7 +2018,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" s="4">
         <v>18</v>
@@ -2046,7 +2050,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B20" s="4">
         <v>19</v>
@@ -2055,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E20" s="4">
         <v>125</v>
@@ -2078,13 +2082,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" s="4">
         <v>20</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>11</v>
@@ -2110,7 +2114,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B22" s="4">
         <v>21</v>
@@ -2142,7 +2146,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B23" s="4">
         <v>22</v>
@@ -2174,7 +2178,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B24" s="4">
         <v>23</v>
@@ -2206,7 +2210,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B25" s="4">
         <v>24</v>
@@ -2238,7 +2242,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B26" s="4">
         <v>25</v>
@@ -2270,7 +2274,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B27" s="4">
         <v>26</v>
@@ -2302,7 +2306,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B28" s="4">
         <v>27</v>
@@ -2334,7 +2338,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B29" s="4">
         <v>28</v>
@@ -2366,7 +2370,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B30" s="4">
         <v>29</v>
@@ -2398,7 +2402,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B31" s="4">
         <v>30</v>
@@ -2430,7 +2434,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B32" s="4">
         <v>31</v>
@@ -2462,7 +2466,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B33" s="4">
         <v>32</v>
@@ -2494,7 +2498,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B34" s="4">
         <v>33</v>
@@ -2526,7 +2530,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B35" s="4">
         <v>34</v>
@@ -2558,7 +2562,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B36" s="4">
         <v>35</v>
@@ -2590,7 +2594,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B37" s="4">
         <v>36</v>
@@ -2622,7 +2626,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B38" s="4">
         <v>37</v>
@@ -2654,7 +2658,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B39" s="4">
         <v>38</v>
@@ -2686,7 +2690,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B40" s="4">
         <v>39</v>
@@ -2701,7 +2705,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G40" s="9">
         <v>15</v>
@@ -2718,7 +2722,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B41" s="4">
         <v>40</v>
@@ -2730,7 +2734,7 @@
         <v>11</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>11</v>
@@ -2750,7 +2754,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B42" s="4">
         <v>41</v>
@@ -2782,7 +2786,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B43" s="4">
         <v>42</v>
@@ -2814,7 +2818,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B44" s="4">
         <v>43</v>
@@ -2846,7 +2850,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B45" s="4">
         <v>44</v>
@@ -2878,7 +2882,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B46" s="4">
         <v>45</v>
@@ -2910,7 +2914,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B47" s="4">
         <v>46</v>
@@ -2942,7 +2946,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B48" s="4">
         <v>47</v>
@@ -2974,7 +2978,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B49" s="4">
         <v>48</v>
@@ -3006,7 +3010,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B50" s="4">
         <v>49</v>
@@ -3038,7 +3042,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B51" s="4">
         <v>50</v>
@@ -3070,7 +3074,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B52" s="4">
         <v>51</v>
@@ -3102,7 +3106,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B53" s="4">
         <v>52</v>
@@ -3134,7 +3138,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B54" s="4">
         <v>53</v>
@@ -3166,7 +3170,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B55" s="4">
         <v>54</v>
@@ -3198,7 +3202,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B56" s="4">
         <v>55</v>
@@ -3230,7 +3234,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B57" s="4">
         <v>56</v>
@@ -3262,7 +3266,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B58" s="4">
         <v>57</v>
@@ -3294,7 +3298,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B59" s="4">
         <v>58</v>
@@ -3326,7 +3330,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B60" s="4">
         <v>59</v>
@@ -3358,7 +3362,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B61" s="4">
         <v>60</v>
@@ -3390,7 +3394,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B62" s="4">
         <v>61</v>
@@ -3422,7 +3426,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B63" s="4">
         <v>62</v>
@@ -3454,7 +3458,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B64" s="4">
         <v>63</v>
@@ -3486,7 +3490,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B65" s="4">
         <v>64</v>
@@ -3518,7 +3522,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B66" s="4">
         <v>65</v>
@@ -3550,7 +3554,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B67" s="4">
         <v>66</v>
@@ -3582,7 +3586,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B68" s="4">
         <v>67</v>
@@ -3603,7 +3607,7 @@
         <v>0</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I68" s="4">
         <v>400</v>
@@ -3614,7 +3618,7 @@
     </row>
     <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B69" s="5">
         <v>68</v>
@@ -3622,7 +3626,7 @@
       <c r="C69" s="5">
         <v>200</v>
       </c>
-      <c r="D69" s="36" t="s">
+      <c r="D69" s="35" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="5">
@@ -3631,8 +3635,8 @@
       <c r="F69" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G69" s="37" t="s">
-        <v>26</v>
+      <c r="G69" s="36" t="s">
+        <v>24</v>
       </c>
       <c r="H69" s="15">
         <v>0</v>

</xml_diff>